<commit_message>
Adapt workflow for first Eurofins submission
</commit_message>
<xml_diff>
--- a/data/parameter_unit_mapping.xlsx
+++ b/data/parameter_unit_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Oeyvind_G\Tiltaksovervakingen\tiltaksovervakingen\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636C7FEB-BDFA-4974-BE1C-5074795AD51F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7257169-A31D-40A9-96A5-8937D648AA0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2C95D8C2-1D7D-4BE6-876F-4C730C778911}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <author>tc={96515918-C46F-42F1-B156-BFEB43DAC499}</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{96F00C65-26B7-4071-9983-247EEBF12006}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{96F00C65-26B7-4071-9983-247EEBF12006}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -46,7 +46,7 @@
     In Vannmiljø units</t>
       </text>
     </comment>
-    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{D33EE2BD-98B9-4FC7-A52F-1550500BC5A2}">
+    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{D33EE2BD-98B9-4FC7-A52F-1550500BC5A2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -54,7 +54,7 @@
     In Vannmiljø units</t>
       </text>
     </comment>
-    <comment ref="H4" authorId="2" shapeId="0" xr:uid="{96515918-C46F-42F1-B156-BFEB43DAC499}">
+    <comment ref="K4" authorId="2" shapeId="0" xr:uid="{96515918-C46F-42F1-B156-BFEB43DAC499}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>Temp</t>
   </si>
@@ -210,9 +210,6 @@
     <t>µg/l Si</t>
   </si>
   <si>
-    <t>vl_to_vm_conv_fac</t>
-  </si>
-  <si>
     <t>enh</t>
   </si>
   <si>
@@ -261,12 +258,6 @@
     <t>&lt;ubenevnt&gt;</t>
   </si>
   <si>
-    <t>vestfold_lab_name</t>
-  </si>
-  <si>
-    <t>vestfold_lab_unit</t>
-  </si>
-  <si>
     <t>vannmiljo_name</t>
   </si>
   <si>
@@ -280,6 +271,27 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>eurofins_name</t>
+  </si>
+  <si>
+    <t>eurofins_unit</t>
+  </si>
+  <si>
+    <t>eurofins_to_vm_conv_fac</t>
+  </si>
+  <si>
+    <t>ms/m</t>
+  </si>
+  <si>
+    <t>vestfoldlab_name</t>
+  </si>
+  <si>
+    <t>vestfoldlab_unit</t>
+  </si>
+  <si>
+    <t>vestfoldlab_to_vm_conv_fac</t>
   </si>
 </sst>
 </file>
@@ -290,7 +302,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,12 +317,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -663,13 +669,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G1" dT="2020-09-29T09:32:04.66" personId="{2A2FE5C0-3DAF-46EB-9168-FBBE27685198}" id="{96F00C65-26B7-4071-9983-247EEBF12006}">
+  <threadedComment ref="J1" dT="2020-09-29T09:32:04.66" personId="{2A2FE5C0-3DAF-46EB-9168-FBBE27685198}" id="{96F00C65-26B7-4071-9983-247EEBF12006}">
     <text>In Vannmiljø units</text>
   </threadedComment>
-  <threadedComment ref="H1" dT="2020-09-29T09:32:11.07" personId="{2A2FE5C0-3DAF-46EB-9168-FBBE27685198}" id="{D33EE2BD-98B9-4FC7-A52F-1550500BC5A2}">
+  <threadedComment ref="K1" dT="2020-09-29T09:32:11.07" personId="{2A2FE5C0-3DAF-46EB-9168-FBBE27685198}" id="{D33EE2BD-98B9-4FC7-A52F-1550500BC5A2}">
     <text>In Vannmiljø units</text>
   </threadedComment>
-  <threadedComment ref="H4" dT="2020-11-04T11:42:09.87" personId="{2A2FE5C0-3DAF-46EB-9168-FBBE27685198}" id="{96515918-C46F-42F1-B156-BFEB43DAC499}">
+  <threadedComment ref="K4" dT="2020-11-04T11:42:09.87" personId="{2A2FE5C0-3DAF-46EB-9168-FBBE27685198}" id="{96515918-C46F-42F1-B156-BFEB43DAC499}">
     <text>See e-mail from Øyvind G received 13.10.2020 at 11.14</text>
   </threadedComment>
 </ThreadedComments>
@@ -677,54 +683,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF985D1-BBD4-4258-AC25-5AD6C24F8C02}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.46484375" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -738,45 +758,63 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>-10</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -790,19 +828,28 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -816,19 +863,28 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -842,19 +898,28 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
@@ -868,19 +933,28 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
+      <c r="G7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>4000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
@@ -894,14 +968,23 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -920,19 +1003,28 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>45</v>
@@ -946,19 +1038,28 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -972,19 +1073,28 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
@@ -998,19 +1108,28 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
+      <c r="G12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
@@ -1024,14 +1143,23 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1050,19 +1178,28 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
+      <c r="G14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -1076,14 +1213,23 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
+      <c r="G15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1102,19 +1248,28 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -1128,19 +1283,28 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
+      <c r="G17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
@@ -1154,14 +1318,23 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
+      <c r="G18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1181,14 +1354,24 @@
         <f>1000*28.09/60.08</f>
         <v>467.54327563249001</v>
       </c>
-      <c r="G19" s="7">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7">
+      <c r="G19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="8">
+        <f>28.09/60.08</f>
+        <v>0.46754327563249004</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7">
         <v>7000</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1207,10 +1390,19 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20">
         <v>-1000</v>
       </c>
-      <c r="H20">
+      <c r="K20">
         <v>6000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Vannmiljø name for ANC has changed
</commit_message>
<xml_diff>
--- a/data/parameter_unit_mapping.xlsx
+++ b/data/parameter_unit_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Oeyvind_G\Tiltaksovervakingen\tiltaksovervakingen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7257169-A31D-40A9-96A5-8937D648AA0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E395B6-A2C0-462E-938C-66E3DE3BEB1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2C95D8C2-1D7D-4BE6-876F-4C730C778911}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
   <si>
     <t>Temp</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>vestfoldlab_to_vm_conv_fac</t>
+  </si>
+  <si>
+    <t>Syrenøytraliserende kapasitet (ANC)</t>
   </si>
 </sst>
 </file>
@@ -686,12 +689,12 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.06640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
@@ -1373,7 +1376,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Update stations and parameter mappings
</commit_message>
<xml_diff>
--- a/data/parameter_unit_mapping.xlsx
+++ b/data/parameter_unit_mapping.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Oeyvind_G\Tiltaksovervakingen\tiltaksovervakingen\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E395B6-A2C0-462E-938C-66E3DE3BEB1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A730A-9BBF-4962-931C-F8BDB9543C81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2C95D8C2-1D7D-4BE6-876F-4C730C778911}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{2C95D8C2-1D7D-4BE6-876F-4C730C778911}"/>
   </bookViews>
   <sheets>
-    <sheet name="vestfoldlab_to_vannmiljo" sheetId="1" r:id="rId1"/>
+    <sheet name="to_vannmiljo" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -689,25 +689,25 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>63</v>
       </c>
@@ -742,7 +742,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -777,7 +777,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -812,7 +812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -847,7 +847,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -882,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -917,7 +917,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -952,7 +952,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -987,7 +987,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>

</xml_diff>